<commit_message>
Fixed issue #3: Finally wrote some documentation.
</commit_message>
<xml_diff>
--- a/tests/data/test_case_b.xlsx
+++ b/tests/data/test_case_b.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480"/>
@@ -10,7 +10,7 @@
     <sheet name="Nodes" sheetId="1" r:id="rId1"/>
     <sheet name="Lines" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -116,7 +116,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -142,6 +142,22 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -185,9 +201,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -198,7 +218,11 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="6">
+    <cellStyle name="Besuchter Link" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="TableStyleLight1" xfId="1"/>
   </cellStyles>
@@ -573,7 +597,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="1025" width="9.1640625" style="1"/>
@@ -661,7 +685,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -680,7 +704,8 @@
   <cols>
     <col min="1" max="1" width="9.1640625" style="1"/>
     <col min="2" max="3" width="9.5" style="1" customWidth="1"/>
-    <col min="4" max="1027" width="9.1640625" style="1"/>
+    <col min="4" max="4" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="1027" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -840,7 +865,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>